<commit_message>
Additional Properties for Trendlines
Fix #3011. Some properties for Trendlines were omitted in the original request for this feature. Also, the trendlines sample spreadsheet included two charts. The rendering script 35_Chart_render handles this, but overlays the first output file with the second. It is changed to produce files with different names.
</commit_message>
<xml_diff>
--- a/samples/templates/32readwriteScatterChartTrendlines1.xlsx
+++ b/samples/templates/32readwriteScatterChartTrendlines1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rounded\samples\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\trendlines2\samples\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7717E2-981F-41B2-BA36-D1BB9DA67545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAC0152-7F04-490C-9176-C710F7BFA067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,6 +640,7 @@
             <c:dispEq val="0"/>
           </c:trendline>
           <c:trendline>
+            <c:name>metric3 polynomial</c:name>
             <c:spPr>
               <a:ln w="15875">
                 <a:solidFill>
@@ -649,6 +650,9 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
+            <c:forward val="28"/>
+            <c:backward val="20"/>
+            <c:intercept val="14400.5"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>

</xml_diff>

<commit_message>
Additional Properties for Trendlines (#3028)
Fix #3011. Some properties for Trendlines were omitted in the original request for this feature. Also, the trendlines sample spreadsheet included two charts. The rendering script 35_Chart_render handles this, but overlays the first output file with the second. It is changed to produce files with different names.
</commit_message>
<xml_diff>
--- a/samples/templates/32readwriteScatterChartTrendlines1.xlsx
+++ b/samples/templates/32readwriteScatterChartTrendlines1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\rounded\samples\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\trendlines2\samples\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7717E2-981F-41B2-BA36-D1BB9DA67545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAC0152-7F04-490C-9176-C710F7BFA067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,6 +640,7 @@
             <c:dispEq val="0"/>
           </c:trendline>
           <c:trendline>
+            <c:name>metric3 polynomial</c:name>
             <c:spPr>
               <a:ln w="15875">
                 <a:solidFill>
@@ -649,6 +650,9 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
+            <c:forward val="28"/>
+            <c:backward val="20"/>
+            <c:intercept val="14400.5"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>

</xml_diff>